<commit_message>
Popravljeni bugovi, ulepsan kod, dodati komentari
</commit_message>
<xml_diff>
--- a/sample_1.xlsx
+++ b/sample_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sj_ruby_domacizadatak\sj_ruby_domacizadatak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620A4BF8-DF61-4D2A-A45E-0AC0FB0AA4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6FD9B1-D185-408C-92FB-C262646E0095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>header1</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>header4</t>
+  </si>
+  <si>
+    <t>SUBTOTAL</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -80,9 +86,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -380,10 +389,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E9E2DA-4D52-49B7-BD0F-92FC568F0898}">
-  <dimension ref="E23:H28"/>
+  <dimension ref="E23:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,10 +415,10 @@
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E25" s="2">
+      <c r="E25" s="3">
         <v>5</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="3"/>
       <c r="G25" s="1">
         <v>6</v>
       </c>
@@ -421,34 +430,90 @@
       <c r="F26">
         <v>2</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="3">
         <v>7</v>
       </c>
+      <c r="H26" s="3"/>
     </row>
     <row r="27" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E27">
+      <c r="E27" s="3">
         <v>2</v>
       </c>
       <c r="F27">
         <v>6</v>
       </c>
+      <c r="G27" s="2"/>
       <c r="H27">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E28">
-        <f>SUBTOTAL(9, E24:E27)</f>
+      <c r="E28" s="3"/>
+      <c r="G28">
         <v>7</v>
       </c>
-      <c r="G28">
-        <f>SUBTOTAL(9,G24:G27)</f>
-        <v>13</v>
+    </row>
+    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>7</v>
+      </c>
+      <c r="H33">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="E27:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>